<commit_message>
Add function to send excel file to email
</commit_message>
<xml_diff>
--- a/Data/Output/ResultTable.xlsx
+++ b/Data/Output/ResultTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\REF-Invoices\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55DCE72-84EA-471C-A16E-09CC1437B55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB112D-E37A-41DF-83A2-436BBF8DBB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -44,6 +44,24 @@
   </x:si>
   <x:si>
     <x:t>Total Due</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n4zdfr8rz4cdlxzf49uy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>j6qky8ysjflms7kciqj97i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>g15db3dv9zupp579hzbzm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15-07-2024</x:t>
   </x:si>
   <x:si>
     <x:t>284221</x:t>
@@ -406,12 +424,21 @@
   <x:dimension ref="A1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="I12" sqref="I12"/>
+      <x:selection activeCell="C13" sqref="C13"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="22" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="17.554688" style="0" customWidth="1"/>
+    <x:col min="3" max="4" width="15" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.109375" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="9" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="14.332031" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="23.554688" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -430,95 +457,71 @@
       <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
-      <x:c r="C2" s="0" t="s">
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="A4" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="C3" s="0" t="s">
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="C6" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="F6" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="E5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:9">
-      <x:c r="E6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:9">
+    <x:row r="7" spans="1:8">
+      <x:c r="C7" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="C8" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>15</x:v>
+      <x:c r="F8" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>